<commit_message>
Added update excel file
</commit_message>
<xml_diff>
--- a/bim_sample_2022.xlsx
+++ b/bim_sample_2022.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Projectfolder\bim_sample_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1759A191-ECCF-416B-94E6-3B41C5152753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2179941-1C9E-4B92-A5F2-087495C37051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="1125" windowWidth="18210" windowHeight="9000" xr2:uid="{2641298C-5040-429D-B40B-01DB16DACBFF}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="18210" windowHeight="9000" activeTab="1" xr2:uid="{2641298C-5040-429D-B40B-01DB16DACBFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Inputs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -382,6 +383,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12E54669-F48C-47CD-B988-671D29FA718A}">
   <dimension ref="A1"/>
   <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{376203C7-4ED8-40A1-BF7F-1CC361E4772A}">
+  <dimension ref="A1"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>